<commit_message>
Import Products Plugin XmltoXlsx convertion
</commit_message>
<xml_diff>
--- a/src/Plugins/Nop.Plugin.Import.ItLink/products.xlsx
+++ b/src/Plugins/Nop.Plugin.Import.ItLink/products.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
   <si>
     <t>ProductType</t>
   </si>
@@ -308,38 +308,9 @@
     <t>Simple Product</t>
   </si>
   <si>
-    <t>ASRock H81 Pro BTC R2.0 Socket 1150</t>
-  </si>
-  <si>
-    <t>/ Производитель: ASRock
-/ Сокет: Socket 1150
-/ Поддержка памяти: DDR3
-/ Формфактор: ATX</t>
-  </si>
-  <si>
-    <t>&lt;div class="pp-characteristics-tab-i" id="pp-characteristics-tab-i" style="text-align: left;"&gt;
-&lt;p&gt;Возможно, вы еще не задумывались над тем, что ваш компьютер очень боится воды, влаги и любых ее проявлений. Отсутствие прямого контакта с водой еще ничего не означает – невидимая избыточная влага медленно и незаметно уничтожает вашу материнскую плату. Конечно, от влаги ваша плата не растает, но она просто выйдет из строя от короткого замыкания. К счастью, компания ASRock разработала новую конструкцию (High Density Glass Fabric PCB), в которой уменьшены зазоры между печатными платами, что обеспечивает дополнительную защиту от короткого замыкания, вызываемого влажностью.&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;Четырехфазное питание&lt;/b&gt;&lt;/p&gt;
-&lt;p&gt;В отличие от большинства конкурентов, использующих 3-х фазную схему питания, ASRock оснащает свои материнские платы 4-х фазными схемами, конструкция и надежные компоненты которых обеспечивают равномерное питание CPU, что улучшает производительность материнской платы, повышает стабильность и снижает температуру.&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;Твердотельные конденсаторы&lt;/b&gt;&lt;/p&gt;
-&lt;p&gt;Для сборки лучших материнских плат компания ASRock выбирает только высококачественные материалы, и поэтому данная материнская плата на 100% оснащена твердотельными конденсаторами. Такие конденсаторы очень надежны в работе и обеспечивают стабильную производительность.&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;Power&lt;/b&gt;&lt;/p&gt;
-&lt;p&gt;В отличие от обычных плат, где применяются аналоговые схемы питания, в этой плате использована технология цифровой широтно-импульсной модуляции (ШИМ) нового поколения, которая обеспечивает более эффективное и равномерное питание CPU, что значительно повышает стабильность и срок службы материнской платы.&lt;span id="copyinfo"&gt;&lt;br /&gt;&lt;br /&gt;&lt;/span&gt;&lt;/p&gt;
-&lt;/div&gt;</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t>Simple product</t>
   </si>
   <si>
-    <t>asrock-h81-pro-btc-r20-socket-1150</t>
-  </si>
-  <si>
-    <t>H81 PRO BTC R2.0</t>
-  </si>
-  <si>
     <t>Virtual</t>
   </si>
   <si>
@@ -359,18 +330,6 @@
   </si>
   <si>
     <t>kg(s)</t>
-  </si>
-  <si>
-    <t>Материнские платы;Материнские платы;</t>
-  </si>
-  <si>
-    <t>C:\HostingSpaces\antonv\mbnpro.com.ua\wwwroot\content\images\thumbs\0000105_asrock-h81-pro-btc-r20-socket-1150.jpeg</t>
-  </si>
-  <si>
-    <t>C:\HostingSpaces\antonv\mbnpro.com.ua\wwwroot\content\images\thumbs\0000106_asrock-h81-pro-btc-r20-socket-1150.jpeg</t>
-  </si>
-  <si>
-    <t>C:\HostingSpaces\antonv\mbnpro.com.ua\wwwroot\content\images\thumbs\0000104_asrock-h81-pro-btc-r20-socket-1150.jpeg</t>
   </si>
   <si>
     <t>Dont Manage Stock</t>
@@ -762,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CP2"/>
+  <dimension ref="A1:CP1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,253 +1013,11 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>101</v>
-      </c>
-      <c r="S2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>102</v>
-      </c>
-      <c r="V2" t="b">
-        <v>0</v>
-      </c>
-      <c r="X2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB2">
-        <v>10</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AD2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI2">
-        <v>100</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK2">
-        <v>10</v>
-      </c>
-      <c r="AL2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AO2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AT2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AY2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AZ2">
-        <v>0</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BC2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>0</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>106</v>
-      </c>
-      <c r="BF2">
-        <v>1</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BH2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BI2">
-        <v>1</v>
-      </c>
-      <c r="BJ2">
-        <v>10000</v>
-      </c>
-      <c r="BL2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BM2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BN2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BO2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BP2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BR2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BS2">
-        <v>155</v>
-      </c>
-      <c r="BT2">
-        <v>0</v>
-      </c>
-      <c r="BU2">
-        <v>0</v>
-      </c>
-      <c r="BV2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BW2">
-        <v>0</v>
-      </c>
-      <c r="BX2">
-        <v>1000</v>
-      </c>
-      <c r="BY2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BZ2">
-        <v>0</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>108</v>
-      </c>
-      <c r="CB2">
-        <v>0</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>108</v>
-      </c>
-      <c r="CD2" t="b">
-        <v>0</v>
-      </c>
-      <c r="CG2">
-        <v>0</v>
-      </c>
-      <c r="CH2">
-        <v>0</v>
-      </c>
-      <c r="CI2">
-        <v>0</v>
-      </c>
-      <c r="CJ2">
-        <v>0</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>109</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>110</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>111</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>112</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="462">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="462">
         <x14:dataValidation type="list">
           <x14:formula1>
             <xm:f>DataForProductsFilters!A1:A2</xm:f>
@@ -4092,118 +3809,118 @@
         <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="H1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="T1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CA1" t="s">
         <v>102</v>
       </c>
-      <c r="AC1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>116</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>106</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>107</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>108</v>
-      </c>
       <c r="CC1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA2" t="s">
         <v>117</v>
       </c>
-      <c r="G2" t="s">
-        <v>118</v>
-      </c>
-      <c r="H2" t="s">
-        <v>119</v>
-      </c>
-      <c r="T2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>124</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>125</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>126</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>127</v>
-      </c>
       <c r="CC2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="AJ3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="AN3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="AS3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="AW3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="AX3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="BE3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="BG3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="AJ4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="AN4" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>